<commit_message>
update kieu du lieu export cho chuc nang export excel
</commit_message>
<xml_diff>
--- a/server/upload/human-resource/templateImport/templateImportHoliday.xlsx
+++ b/server/upload/human-resource/templateImport/templateImportHoliday.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hung Cuong\Desktop\qlcv\server\upload\human-resource\templateImport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C452DACC-2107-4A23-9244-0D980414A891}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D34A74-173F-4D25-8762-6245E5C5CECE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -435,16 +435,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>723900</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3867150</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>139514</xdr:rowOff>
+      <xdr:rowOff>129989</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -459,8 +459,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2714625" y="790575"/>
-          <a:ext cx="3648075" cy="301439"/>
+          <a:off x="657225" y="781050"/>
+          <a:ext cx="7086600" cy="301439"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -494,7 +494,7 @@
               <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:rPr>
-            <a:t>KẾ HOẠCH LÀM VIỆC</a:t>
+            <a:t>MẪU IMPORT KẾ HOẠCH LÀM VIỆC</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -770,7 +770,7 @@
   <dimension ref="A1:F2422"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>